<commit_message>
- add five [A] ballots and one [E,A] ballot to shared bottoms_up_cvr.xlsx - update bottoms up with percentage threshold static and dynamic test expected results
</commit_message>
<xml_diff>
--- a/src/test/resources/network/brightspots/rcv/test_data/_shared/bottoms_up_cvr.xlsx
+++ b/src/test/resources/network/brightspots/rcv/test_data/_shared/bottoms_up_cvr.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yezr/localrepo/rctab_github/rcv/src/test/resources/network/brightspots/rcv/test_data/_shared/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5EE7E5E-9AC3-6E4D-80D5-BD20C56AE754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="-24540" yWindow="4800" windowWidth="23200" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="8">
   <si>
     <t>A</t>
   </si>
@@ -40,25 +49,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -94,26 +90,14 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -122,23 +106,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -340,7 +386,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -359,7 +405,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -389,7 +435,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -415,7 +461,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -441,7 +487,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -467,7 +513,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -493,7 +539,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -519,7 +565,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -545,7 +591,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -571,7 +617,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -597,7 +643,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -610,9 +656,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -629,7 +681,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -648,7 +700,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -674,7 +726,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -700,7 +752,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -726,7 +778,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -752,7 +804,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -778,7 +830,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -804,7 +856,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -830,7 +882,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -856,7 +908,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -882,7 +934,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -895,9 +947,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -911,7 +969,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -930,7 +988,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -960,7 +1018,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -986,7 +1044,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1012,7 +1070,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1038,7 +1096,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1064,7 +1122,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1090,7 +1148,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1116,7 +1174,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1142,7 +1200,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1168,7 +1226,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1181,32 +1239,41 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="6" width="14.5" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="14.5" style="1" customWidth="1"/>
+    <col min="1" max="7" width="14.5" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="14.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.65" customHeight="1">
+    <row r="1" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2"/>
       <c r="B1" s="3">
         <v>1</v>
@@ -1224,409 +1291,409 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" ht="13.65" customHeight="1">
+    <row r="2" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="4">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s" s="4">
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s" s="4">
+      <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" ht="13.65" customHeight="1">
+      <c r="E2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" t="s" s="4">
+      <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C3" t="s" s="4">
+      <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" t="s" s="4">
+      <c r="D3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E3" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="F3" t="s" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" ht="13.65" customHeight="1">
+      <c r="E3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" t="s" s="4">
+      <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" t="s" s="4">
+      <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" t="s" s="4">
+      <c r="D4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="F4" t="s" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" ht="13.65" customHeight="1">
+      <c r="E4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" t="s" s="4">
+      <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C5" t="s" s="4">
+      <c r="C5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D5" t="s" s="4">
+      <c r="D5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E5" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="F5" t="s" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" ht="13.65" customHeight="1">
+      <c r="E5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" t="s" s="4">
+      <c r="B6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C6" t="s" s="4">
+      <c r="C6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D6" t="s" s="4">
+      <c r="D6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E6" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="F6" t="s" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" ht="13.65" customHeight="1">
+      <c r="E6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" t="s" s="4">
+      <c r="B7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C7" t="s" s="4">
+      <c r="C7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D7" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="E7" t="s" s="4">
-        <v>4</v>
-      </c>
-      <c r="F7" t="s" s="4">
+      <c r="D7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" ht="13.65" customHeight="1">
+    <row r="8" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" t="s" s="4">
+      <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C8" t="s" s="4">
+      <c r="C8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D8" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="E8" t="s" s="4">
-        <v>4</v>
-      </c>
-      <c r="F8" t="s" s="4">
+      <c r="D8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" ht="13.65" customHeight="1">
+    <row r="9" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" t="s" s="4">
+      <c r="B9" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C9" t="s" s="4">
+      <c r="C9" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D9" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="E9" t="s" s="4">
-        <v>4</v>
-      </c>
-      <c r="F9" t="s" s="4">
+      <c r="D9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" ht="13.65" customHeight="1">
+    <row r="10" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" t="s" s="4">
+      <c r="B10" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C10" t="s" s="4">
+      <c r="C10" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D10" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="E10" t="s" s="4">
-        <v>4</v>
-      </c>
-      <c r="F10" t="s" s="4">
+      <c r="D10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" ht="13.65" customHeight="1">
+    <row r="11" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" t="s" s="4">
+      <c r="B11" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C11" t="s" s="4">
+      <c r="C11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D11" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="E11" t="s" s="4">
-        <v>4</v>
-      </c>
-      <c r="F11" t="s" s="4">
+      <c r="D11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" ht="13.65" customHeight="1">
+    <row r="12" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" t="s" s="4">
+      <c r="B12" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C12" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="D12" t="s" s="4">
-        <v>4</v>
-      </c>
-      <c r="E12" t="s" s="4">
+      <c r="C12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F12" t="s" s="4">
+      <c r="F12" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" ht="13.65" customHeight="1">
+    <row r="13" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13" t="s" s="4">
+      <c r="B13" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C13" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="D13" t="s" s="4">
-        <v>4</v>
-      </c>
-      <c r="E13" t="s" s="4">
+      <c r="C13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F13" t="s" s="4">
+      <c r="F13" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" ht="13.65" customHeight="1">
+    <row r="14" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14" t="s" s="4">
+      <c r="B14" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C14" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="D14" t="s" s="4">
-        <v>4</v>
-      </c>
-      <c r="E14" t="s" s="4">
+      <c r="C14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F14" t="s" s="4">
+      <c r="F14" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" ht="13.65" customHeight="1">
+    <row r="15" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
         <v>14</v>
       </c>
-      <c r="B15" t="s" s="4">
+      <c r="B15" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C15" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="D15" t="s" s="4">
-        <v>4</v>
-      </c>
-      <c r="E15" t="s" s="4">
+      <c r="C15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F15" t="s" s="4">
+      <c r="F15" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" ht="13.65" customHeight="1">
+    <row r="16" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B16" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="C16" t="s" s="4">
-        <v>4</v>
-      </c>
-      <c r="D16" t="s" s="4">
+      <c r="B16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E16" t="s" s="4">
+      <c r="E16" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F16" t="s" s="4">
+      <c r="F16" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" ht="13.65" customHeight="1">
+    <row r="17" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="3">
         <v>16</v>
       </c>
-      <c r="B17" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="C17" t="s" s="4">
-        <v>4</v>
-      </c>
-      <c r="D17" t="s" s="4">
+      <c r="B17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E17" t="s" s="4">
+      <c r="E17" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F17" t="s" s="4">
+      <c r="F17" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" ht="13.65" customHeight="1">
+    <row r="18" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="3">
         <v>17</v>
       </c>
-      <c r="B18" t="s" s="4">
-        <v>3</v>
-      </c>
-      <c r="C18" t="s" s="4">
-        <v>4</v>
-      </c>
-      <c r="D18" t="s" s="4">
+      <c r="B18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E18" t="s" s="4">
+      <c r="E18" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F18" t="s" s="4">
+      <c r="F18" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" ht="13.65" customHeight="1">
+    <row r="19" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="3">
         <v>18</v>
       </c>
-      <c r="B19" t="s" s="4">
+      <c r="B19" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C19" t="s" s="4">
+      <c r="C19" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D19" t="s" s="4">
+      <c r="D19" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" ht="13.65" customHeight="1">
+    <row r="20" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="3">
         <v>19</v>
       </c>
-      <c r="B20" t="s" s="4">
+      <c r="B20" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C20" t="s" s="4">
+      <c r="C20" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" ht="13.65" customHeight="1">
+    <row r="21" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="3">
         <v>20</v>
       </c>
-      <c r="B21" t="s" s="4">
+      <c r="B21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C21" t="s" s="4">
+      <c r="C21" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" ht="13.65" customHeight="1">
+    <row r="22" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="3">
         <v>21</v>
       </c>
-      <c r="B22" t="s" s="4">
+      <c r="B22" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C22" t="s" s="4">
+      <c r="C22" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" ht="13.65" customHeight="1">
+    <row r="23" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="3">
         <v>22</v>
       </c>
-      <c r="B23" t="s" s="4">
+      <c r="B23" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C23" s="2"/>
@@ -1634,9 +1701,71 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="2">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="2">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="2">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>